<commit_message>
Recruitment and risk analysis correction
</commit_message>
<xml_diff>
--- a/programs/recruitment/Recruitment Model Inputs 1997-2018.xlsx
+++ b/programs/recruitment/Recruitment Model Inputs 1997-2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="27795" windowHeight="11820" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="27795" windowHeight="11820" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="R-1" sheetId="2" r:id="rId1"/>
@@ -650,7 +650,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -724,6 +724,7 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1073,7 +1074,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2360,7 +2361,7 @@
       <c r="F25" s="26">
         <v>101882.4</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="31">
         <v>353</v>
       </c>
       <c r="H25" s="25">
@@ -2414,10 +2415,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q25"/>
+      <selection activeCell="Q24" sqref="P24:Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,7 +2510,7 @@
       <c r="G2" s="3">
         <v>254</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="19">
         <v>59731832.780000001</v>
       </c>
       <c r="I2" s="3">
@@ -2561,7 +2562,7 @@
       <c r="G3" s="3">
         <v>256</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="19">
         <v>60327460.899999999</v>
       </c>
       <c r="I3" s="3">
@@ -2613,7 +2614,7 @@
       <c r="G4" s="3">
         <v>273</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="19">
         <v>112947093.59999999</v>
       </c>
       <c r="I4" s="3">
@@ -2665,7 +2666,7 @@
       <c r="G5" s="3">
         <v>275</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="19">
         <v>88449623.329999998</v>
       </c>
       <c r="I5" s="3">
@@ -2717,7 +2718,7 @@
       <c r="G6" s="3">
         <v>287</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="19">
         <v>136263321.59999999</v>
       </c>
       <c r="I6" s="3">
@@ -2769,7 +2770,7 @@
       <c r="G7" s="3">
         <v>311</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="19">
         <v>202195282.69999999</v>
       </c>
       <c r="I7" s="3">
@@ -2821,7 +2822,7 @@
       <c r="G8" s="3">
         <v>308</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="19">
         <v>178485325.09999999</v>
       </c>
       <c r="I8" s="3">
@@ -2873,7 +2874,7 @@
       <c r="G9" s="3">
         <v>332</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="19">
         <v>144090400</v>
       </c>
       <c r="I9" s="3">
@@ -2925,7 +2926,7 @@
       <c r="G10" s="3">
         <v>339</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="19">
         <v>117190599.40000001</v>
       </c>
       <c r="I10" s="3">
@@ -2977,7 +2978,7 @@
       <c r="G11" s="3">
         <v>348</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="19">
         <v>65680337.659999996</v>
       </c>
       <c r="I11" s="3">
@@ -3029,7 +3030,7 @@
       <c r="G12" s="3">
         <v>348</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="19">
         <v>55449964.289999999</v>
       </c>
       <c r="I12" s="3">
@@ -3081,7 +3082,7 @@
       <c r="G13" s="3">
         <v>349</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="19">
         <v>45841439.240000002</v>
       </c>
       <c r="I13" s="3">
@@ -3133,7 +3134,7 @@
       <c r="G14" s="3">
         <v>349</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="19">
         <v>43791209.219999999</v>
       </c>
       <c r="I14" s="3">
@@ -3185,7 +3186,7 @@
       <c r="G15" s="3">
         <v>347</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="19">
         <v>72543724.799999997</v>
       </c>
       <c r="I15" s="3">
@@ -3237,7 +3238,7 @@
       <c r="G16" s="3">
         <v>347</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="19">
         <v>88179433.25</v>
       </c>
       <c r="I16" s="3">
@@ -3289,7 +3290,7 @@
       <c r="G17" s="3">
         <v>321</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="19">
         <v>80509186.5</v>
       </c>
       <c r="I17" s="3">
@@ -3341,7 +3342,7 @@
       <c r="G18" s="3">
         <v>352</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="19">
         <v>79432086.959999993</v>
       </c>
       <c r="I18" s="3">
@@ -3393,7 +3394,7 @@
       <c r="G19" s="3">
         <v>353</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="19">
         <v>117187112.7</v>
       </c>
       <c r="I19" s="3">
@@ -3445,7 +3446,7 @@
       <c r="G20" s="3">
         <v>352</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="19">
         <v>127476371.90000001</v>
       </c>
       <c r="I20" s="3">
@@ -3497,7 +3498,7 @@
       <c r="G21" s="3">
         <v>354</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="19">
         <v>101572651.3</v>
       </c>
       <c r="I21" s="3">
@@ -3549,7 +3550,7 @@
       <c r="G22" s="3">
         <v>353</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="19">
         <v>103308656.09999999</v>
       </c>
       <c r="I22" s="3">
@@ -3601,7 +3602,7 @@
       <c r="G23" s="3">
         <v>354</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="19">
         <v>108305804.90000001</v>
       </c>
       <c r="I23" s="3">
@@ -3653,34 +3654,34 @@
       <c r="G24" s="6">
         <v>352</v>
       </c>
-      <c r="H24" s="6">
-        <v>163872847</v>
+      <c r="H24" s="27">
+        <v>185661294.229334</v>
       </c>
       <c r="I24" s="6">
-        <v>14461268</v>
+        <v>16045922.072286401</v>
       </c>
       <c r="J24" s="6">
-        <v>137357461</v>
+        <v>156198371.261336</v>
       </c>
       <c r="K24" s="6">
-        <v>193995997</v>
+        <v>219045520.04934898</v>
       </c>
       <c r="L24" s="6">
-        <v>-20.089410000000001</v>
+        <v>-28.769196033405198</v>
       </c>
       <c r="M24" s="6">
-        <v>2601.741</v>
+        <v>2943.69034365775</v>
       </c>
       <c r="N24" s="6">
-        <v>4704.0959999999995</v>
+        <v>5183.2574068902195</v>
       </c>
       <c r="P24" s="8">
         <f t="shared" ref="P24" si="2">LN((H24^2/(SQRT(I24^2+H24^2)))/1000000)</f>
-        <v>5.0952121308132767</v>
+        <v>5.2202031862057483</v>
       </c>
       <c r="Q24" s="12">
         <f t="shared" ref="Q24" si="3">SQRT(LN(1+(I24^2)/(H24^2)))</f>
-        <v>8.8075798284593054E-2</v>
+        <v>8.6265041663367084E-2</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -3705,7 +3706,7 @@
       <c r="G25" s="3">
         <v>353</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="19">
         <v>202980288.66017699</v>
       </c>
       <c r="I25" s="3">
@@ -3738,6 +3739,23 @@
       <c r="P26" s="8"/>
       <c r="Q26" s="12"/>
     </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3749,7 +3767,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q25"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5126,7 +5144,7 @@
       <c r="G25" s="25">
         <v>353</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="27">
         <v>170349373.43262899</v>
       </c>
       <c r="I25" s="25">
@@ -5275,8 +5293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6671,8 +6689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6778,7 +6796,7 @@
       <c r="D3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="13">
         <v>0.10151290707686225</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -6829,10 +6847,10 @@
       <c r="D4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="13">
         <v>0.14701113898528578</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="12">
         <v>0.11031839241074115</v>
       </c>
       <c r="H4" s="6" t="s">
@@ -6880,10 +6898,10 @@
       <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="13">
         <v>0.11312253493828546</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <v>0.12083664322036108</v>
       </c>
       <c r="H5" s="12">
@@ -6932,10 +6950,10 @@
         <v>4.7305128053520074</v>
       </c>
       <c r="E6" s="21"/>
-      <c r="F6">
+      <c r="F6" s="13">
         <v>9.60075327862637E-2</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>0.12864074115937241</v>
       </c>
       <c r="H6" s="12">
@@ -6984,10 +7002,10 @@
         <v>4.9018239672763091</v>
       </c>
       <c r="E7" s="21"/>
-      <c r="F7">
+      <c r="F7" s="13">
         <v>0.11195968788838956</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <v>0.10120367392046674</v>
       </c>
       <c r="H7" s="12">
@@ -7036,10 +7054,10 @@
         <v>5.2698686707255664</v>
       </c>
       <c r="E8" s="21"/>
-      <c r="F8">
+      <c r="F8" s="13">
         <v>8.7795072887129885E-2</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <v>9.3653404932871789E-2</v>
       </c>
       <c r="H8" s="12">
@@ -7088,10 +7106,10 @@
         <v>5.4642199610831961</v>
       </c>
       <c r="E9" s="21"/>
-      <c r="F9">
+      <c r="F9" s="13">
         <v>7.3954027379562096E-2</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <v>8.3595608931868709E-2</v>
       </c>
       <c r="H9" s="12">
@@ -7140,10 +7158,10 @@
         <v>5.7331040562576003</v>
       </c>
       <c r="E10" s="21"/>
-      <c r="F10">
+      <c r="F10" s="13">
         <v>5.9631585616718906E-2</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <v>7.8295092227036234E-2</v>
       </c>
       <c r="H10" s="12">
@@ -7192,10 +7210,10 @@
         <v>5.0963838471238656</v>
       </c>
       <c r="E11" s="21"/>
-      <c r="F11">
+      <c r="F11" s="13">
         <v>5.6643457225994134E-2</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="12">
         <v>7.2783038092628025E-2</v>
       </c>
       <c r="H11" s="12">
@@ -7244,10 +7262,10 @@
         <v>4.8846365259369637</v>
       </c>
       <c r="E12" s="21"/>
-      <c r="F12">
+      <c r="F12" s="13">
         <v>6.1723816387342548E-2</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="12">
         <v>8.2242584667787402E-2</v>
       </c>
       <c r="H12" s="12">
@@ -7296,10 +7314,10 @@
         <v>4.4473914938858163</v>
       </c>
       <c r="E13" s="21"/>
-      <c r="F13">
+      <c r="F13" s="13">
         <v>6.3552412526859225E-2</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="12">
         <v>8.9490928748166707E-2</v>
       </c>
       <c r="H13" s="12">
@@ -7348,10 +7366,10 @@
         <v>4.1262658822768348</v>
       </c>
       <c r="E14" s="21"/>
-      <c r="F14">
+      <c r="F14" s="13">
         <v>7.194219552052683E-2</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="12">
         <v>8.7795972616699802E-2</v>
       </c>
       <c r="H14" s="12">
@@ -7400,10 +7418,10 @@
         <v>3.9856231519217253</v>
       </c>
       <c r="E15" s="21"/>
-      <c r="F15">
+      <c r="F15" s="13">
         <v>7.5048439818444543E-2</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="12">
         <v>0.11264142018988516</v>
       </c>
       <c r="H15" s="12">
@@ -7452,10 +7470,10 @@
         <v>4.0311342277358078</v>
       </c>
       <c r="E16" s="21"/>
-      <c r="F16">
+      <c r="F16" s="13">
         <v>6.9811423626372743E-2</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="12">
         <v>0.1096812133475602</v>
       </c>
       <c r="H16" s="12">
@@ -7504,10 +7522,10 @@
         <v>4.3858035585477833</v>
       </c>
       <c r="E17" s="21"/>
-      <c r="F17">
+      <c r="F17" s="13">
         <v>7.1968781724217903E-2</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="12">
         <v>9.5785735146548132E-2</v>
       </c>
       <c r="H17" s="12">
@@ -7556,10 +7574,10 @@
         <v>4.4802747398742637</v>
       </c>
       <c r="E18" s="21"/>
-      <c r="F18">
+      <c r="F18" s="13">
         <v>9.6425093293823538E-2</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="12">
         <v>6.6927451913130265E-2</v>
       </c>
       <c r="H18" s="12">
@@ -7608,10 +7626,10 @@
         <v>4.9459777797934628</v>
       </c>
       <c r="E19" s="21"/>
-      <c r="F19">
+      <c r="F19" s="13">
         <v>0.11811896894485545</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="12">
         <v>9.1832208796323186E-2</v>
       </c>
       <c r="H19" s="12">
@@ -7660,10 +7678,10 @@
         <v>4.5128210054546098</v>
       </c>
       <c r="E20" s="21"/>
-      <c r="F20">
+      <c r="F20" s="13">
         <v>8.3871516453384767E-2</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="12">
         <v>0.10215224322602443</v>
       </c>
       <c r="H20" s="12">
@@ -7712,10 +7730,10 @@
         <v>4.55697725031846</v>
       </c>
       <c r="E21" s="21"/>
-      <c r="F21">
+      <c r="F21" s="13">
         <v>9.1037443648043989E-2</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="12">
         <v>0.10324574735842106</v>
       </c>
       <c r="H21" s="12">
@@ -7764,10 +7782,10 @@
         <v>4.6311552324257272</v>
       </c>
       <c r="E22" s="21"/>
-      <c r="F22">
+      <c r="F22" s="13">
         <v>6.7346706435741713E-2</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="12">
         <v>8.6541976550571234E-2</v>
       </c>
       <c r="H22" s="12">
@@ -7816,10 +7834,10 @@
         <v>4.6494947862260805</v>
       </c>
       <c r="E23" s="21"/>
-      <c r="F23">
+      <c r="F23" s="13">
         <v>7.5420670265482978E-2</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="12">
         <v>6.6611254757506427E-2</v>
       </c>
       <c r="H23" s="12">
@@ -7868,10 +7886,10 @@
         <v>4.6716943372379909</v>
       </c>
       <c r="E24" s="21"/>
-      <c r="F24">
+      <c r="F24" s="13">
         <v>7.0800400857917611E-2</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="12">
         <v>6.972719325056706E-2</v>
       </c>
       <c r="H24" s="12">
@@ -7920,10 +7938,10 @@
         <v>4.7266372096563671</v>
       </c>
       <c r="E25" s="21"/>
-      <c r="F25" s="6">
+      <c r="F25" s="13">
         <v>8.0564759812070549E-2</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G25" s="12">
         <v>7.7214743690985424E-2</v>
       </c>
       <c r="H25" s="12">
@@ -7965,7 +7983,7 @@
         <v>4.064733954943299</v>
       </c>
       <c r="B26" s="12">
-        <v>5.0952121308132767</v>
+        <v>5.2202031862057483</v>
       </c>
       <c r="C26" s="12">
         <v>4.7556508422131056</v>
@@ -7974,11 +7992,11 @@
         <v>4.7246562641573107</v>
       </c>
       <c r="E26" s="21"/>
-      <c r="F26" s="12">
+      <c r="F26" s="13">
         <v>8.0382796691415112E-2</v>
       </c>
-      <c r="G26" s="13">
-        <v>8.8075798284593054E-2</v>
+      <c r="G26" s="12">
+        <v>8.6265041663367084E-2</v>
       </c>
       <c r="H26" s="12">
         <v>6.2168449426132671E-2</v>
@@ -8031,7 +8049,7 @@
       <c r="F27" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="12">
         <v>8.4592298099316676E-2</v>
       </c>
       <c r="H27" s="12">
@@ -8087,7 +8105,7 @@
       <c r="G28" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="12">
         <v>7.045762372818265E-2</v>
       </c>
       <c r="I28" s="13">
@@ -8143,7 +8161,7 @@
       <c r="H29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="13">
         <v>6.1987782056715506E-2</v>
       </c>
     </row>

</xml_diff>